<commit_message>
cambios para manejar tablas en rama norma-mensual
</commit_message>
<xml_diff>
--- a/tabla_a.xlsx
+++ b/tabla_a.xlsx
@@ -8,43 +8,158 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>CODSUM</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>SANDY BEATRIZ DIAZ CAHUA</t>
-  </si>
-  <si>
-    <t>SONIA RITA YARMA CABEZAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALEJANDRO ORMEÑO </t>
-  </si>
-  <si>
-    <t>JULIO EZEQUIEL MARTINEZ GUTIERREZ</t>
-  </si>
-  <si>
-    <t>DELIA ROSELIN MENDOZA MENDOZA</t>
-  </si>
-  <si>
-    <t>ELIZABETH CONCEPCION ANTISANA GARCIA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+  <si>
+    <t>SUMINISTRO</t>
+  </si>
+  <si>
+    <t>NOMBRES</t>
+  </si>
+  <si>
+    <t>REGISTRE DIRECCIÓN</t>
+  </si>
+  <si>
+    <t>NRO INFORME</t>
+  </si>
+  <si>
+    <t>ROSA JULIA GARCIA CARHUAYO</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Tapa Medidor 01098500 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>ISABEL GALVAN CANTORAL</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Tapa Medidor 01060003 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>CLEMENTINA LOVERA VDA. DE FLORES</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Tapa Medidor 01004700 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>MARIA M. TATAJE M.</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 761 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>PEDRO JULIO ESCATE MUÑANTE</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 201 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>ISABEL LEVANO D.</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 823 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>NILTON FELIPE HUAYLLA ZEGARRA</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Tapa Medidor 01002510 0 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>PEDRO MARTINEZ</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Tapa Medidor 01002100 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>MARIA HAYDEE MUÑOZ DE MONTERREY</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 157 C.P. Camino de Reyes SALAS</t>
+  </si>
+  <si>
+    <t>ROSE MARY GONZALES DE GASTELU</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 110 Fundo Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>INVERSIONES EL CATADOR S.A.C.</t>
+  </si>
+  <si>
+    <t>CL (SIN CALLE) Nro. Puerta 102 ..... Sin Barrio Cas. Tres Esquinas , SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>LEONCIO GONZALES M.</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Tapa Medidor 02003700 0 Fundo Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>JORGE CARRASCO P.</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Tapa Medidor 02003800 Cas. Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>CRISTEL ROXANA CARRASCO GONZALES</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 103 Cas. Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>REST.CAMP.LA OLLA DE JUANITA E.I.R.L.</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 121 Cas. Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>ANGELA DE PEÑA</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 360 Cas. Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>JUANA ROSA PEÑA LEVANO</t>
+  </si>
+  <si>
+    <t>MZNA E Nro. Puerta 07 Cas. Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>PABLO MAURO LOPEZ MAYURI</t>
+  </si>
+  <si>
+    <t>MZNA Nro. Puerta 206 Cas. Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>LA CAPILLA DE TRES ESQUINAS</t>
+  </si>
+  <si>
+    <t>MZNA C Nro. Puerta 01 Cas. Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>VERONICA SABINA VASQUEZ MOQUILLAZA</t>
+  </si>
+  <si>
+    <t>MZNA C Nro. Puerta 02 Cas. Tres Esquinas SUBTANJALLA</t>
+  </si>
+  <si>
+    <t>JUAN CARLOS ROMANI QUISPE</t>
+  </si>
+  <si>
+    <t>PSJE LOS JARDINES DEL SUR Nro. Lote 121 Sin Barrio La Venta Baja , SANTIAGO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,23 +168,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,12 +190,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF16365C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -92,30 +210,62 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -125,12 +275,24 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,75 +597,477 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>101090101</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>101069997</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>101001381</v>
-      </c>
-      <c r="B4" s="6" t="s">
+    <row r="2" spans="1:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>101067264</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>700043730</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>101086169</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="D2" s="5">
+        <v>332076</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>101074942</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>101085220</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="D3" s="5">
+        <v>332079</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>101028629</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5">
+        <v>269811</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>101028722</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5">
+        <v>332078</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>101028737</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5">
+        <v>332077</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>101028727</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5">
+        <v>332075</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>101067264</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5">
+        <v>332074</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>101091029</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>332073</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>101028603</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5">
+        <v>332072</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>101055755</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5">
+        <v>332071</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>101056432</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="5">
+        <v>332070</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>700028026</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5">
+        <v>332069</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>101027103</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5">
+        <v>332068</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>101027105</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5">
+        <v>332067</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>101064641</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="5">
+        <v>332066</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>101070480</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="5">
+        <v>332065</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>101027100</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5">
+        <v>332064</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>101062381</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="5">
+        <v>332063</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>101053333</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="5">
+        <v>332062</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>101074948</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="5">
+        <v>332061</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>101061521</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="5">
+        <v>332060</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>700008306</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="5">
+        <v>268940</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>101067264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>101074942</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>101028629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>101028722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>101028737</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>101028727</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>101067264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>101091029</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>101028603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>101055755</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>101056432</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>700028026</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>101027103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>101027105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>101064641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>101070480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>101027100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>101062381</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>101053333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>101074948</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>101061521</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>700008306</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
revisar salida de tabla b
</commit_message>
<xml_diff>
--- a/tabla_a.xlsx
+++ b/tabla_a.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>SUMINISTRO</t>
   </si>
@@ -23,136 +23,70 @@
     <t>NOMBRES</t>
   </si>
   <si>
-    <t>REGISTRE DIRECCIÓN</t>
-  </si>
-  <si>
-    <t>NRO INFORME</t>
-  </si>
-  <si>
     <t>ROSA JULIA GARCIA CARHUAYO</t>
   </si>
   <si>
-    <t>MZNA Nro. Tapa Medidor 01098500 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>ISABEL GALVAN CANTORAL</t>
   </si>
   <si>
-    <t>MZNA Nro. Tapa Medidor 01060003 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>CLEMENTINA LOVERA VDA. DE FLORES</t>
   </si>
   <si>
-    <t>MZNA Nro. Tapa Medidor 01004700 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>MARIA M. TATAJE M.</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 761 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>PEDRO JULIO ESCATE MUÑANTE</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 201 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>ISABEL LEVANO D.</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 823 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>NILTON FELIPE HUAYLLA ZEGARRA</t>
   </si>
   <si>
-    <t>MZNA Nro. Tapa Medidor 01002510 0 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>PEDRO MARTINEZ</t>
   </si>
   <si>
-    <t>MZNA Nro. Tapa Medidor 01002100 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>MARIA HAYDEE MUÑOZ DE MONTERREY</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 157 C.P. Camino de Reyes SALAS</t>
-  </si>
-  <si>
     <t>ROSE MARY GONZALES DE GASTELU</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 110 Fundo Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>INVERSIONES EL CATADOR S.A.C.</t>
   </si>
   <si>
-    <t>CL (SIN CALLE) Nro. Puerta 102 ..... Sin Barrio Cas. Tres Esquinas , SUBTANJALLA</t>
-  </si>
-  <si>
     <t>LEONCIO GONZALES M.</t>
   </si>
   <si>
-    <t>MZNA Nro. Tapa Medidor 02003700 0 Fundo Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>JORGE CARRASCO P.</t>
   </si>
   <si>
-    <t>MZNA Nro. Tapa Medidor 02003800 Cas. Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>CRISTEL ROXANA CARRASCO GONZALES</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 103 Cas. Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>REST.CAMP.LA OLLA DE JUANITA E.I.R.L.</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 121 Cas. Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>ANGELA DE PEÑA</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 360 Cas. Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>JUANA ROSA PEÑA LEVANO</t>
   </si>
   <si>
-    <t>MZNA E Nro. Puerta 07 Cas. Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>PABLO MAURO LOPEZ MAYURI</t>
   </si>
   <si>
-    <t>MZNA Nro. Puerta 206 Cas. Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>LA CAPILLA DE TRES ESQUINAS</t>
   </si>
   <si>
-    <t>MZNA C Nro. Puerta 01 Cas. Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>VERONICA SABINA VASQUEZ MOQUILLAZA</t>
   </si>
   <si>
-    <t>MZNA C Nro. Puerta 02 Cas. Tres Esquinas SUBTANJALLA</t>
-  </si>
-  <si>
     <t>JUAN CARLOS ROMANI QUISPE</t>
   </si>
   <si>
-    <t>PSJE LOS JARDINES DEL SUR Nro. Lote 121 Sin Barrio La Venta Baja , SANTIAGO</t>
+    <t>NUMEROFICHA</t>
   </si>
 </sst>
 </file>
@@ -597,340 +531,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="3" max="3" width="17.28515625" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>101067264</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
         <v>332076</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>101074942</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5">
         <v>332079</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>101028629</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
         <v>269811</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>101028722</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5">
         <v>332078</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>101028737</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5">
         <v>332077</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>101028727</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5">
         <v>332075</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>101067264</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5">
         <v>332074</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>101091029</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5">
         <v>332073</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>101028603</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="5">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5">
         <v>332072</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>101055755</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5">
         <v>332071</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>101056432</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="5">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5">
         <v>332070</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>700028026</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5">
         <v>332069</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>101027103</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="5">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5">
         <v>332068</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>101027105</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="5">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5">
         <v>332067</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>101064641</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="5">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5">
         <v>332066</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>101070480</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="5">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5">
         <v>332065</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>101027100</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="5">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5">
         <v>332064</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>101062381</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="5">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5">
         <v>332063</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>101053333</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="5">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5">
         <v>332062</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>101074948</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="5">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5">
         <v>332061</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>101061521</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="5">
+        <v>21</v>
+      </c>
+      <c r="C22" s="5">
         <v>332060</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>700008306</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="5">
+        <v>22</v>
+      </c>
+      <c r="C23" s="5">
         <v>268940</v>
       </c>
     </row>

</xml_diff>